<commit_message>
got addition to excel sheet to work
</commit_message>
<xml_diff>
--- a/infoTable.xlsx
+++ b/infoTable.xlsx
@@ -33,6 +33,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>jill</t>
+  </si>
+  <si>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>jackson</t>
+  </si>
+  <si>
+    <t>555-444-3333</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,12 +434,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CBEB51-D6AD-2445-98E5-F175F1EDC462}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>